<commit_message>
Deleting tickets fixing fixture
</commit_message>
<xml_diff>
--- a/fixture/ManCity.xlsx
+++ b/fixture/ManCity.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Manchester City v RB Leipzig</t>
   </si>
@@ -22,138 +22,147 @@
     <t>15/09/2021 20:00 | UEFA Champions League</t>
   </si>
   <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manchester City v Southampton </t>
+  </si>
+  <si>
+    <t>18/09/2021 15:00 | Premier League</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>Manchester City v Wycombe Wanderers</t>
+  </si>
+  <si>
+    <t>21/09/2021 19:45 | Carabao Cup</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>Chelsea v Manchester City</t>
+  </si>
+  <si>
+    <t>25/09/2021 12:30 | Premier League</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>Manchester City v Burnley</t>
+  </si>
+  <si>
+    <t>16/10/2021 15:00 | Premier League</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manchester City v Crystal Palace </t>
+  </si>
+  <si>
+    <t>30/10/2021 15:00 | Premier League</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manchester City v Everton </t>
+  </si>
+  <si>
+    <t>20/11/2021 15:00 | Premier League</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>Manchester City v West Ham United</t>
+  </si>
+  <si>
+    <t>27/11/2021 15:00 | Premier League</t>
+  </si>
+  <si>
+    <t>Manchester City v Wolverhampton Wanderers</t>
+  </si>
+  <si>
+    <t>11/12/2021 15:00 | Premier League</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manchester City v Leeds United </t>
+  </si>
+  <si>
+    <t>15/12/2021 20:00 | Premier League</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>Manchester City v Leicester City</t>
+  </si>
+  <si>
+    <t>26/12/2021 15:00 | Premier League</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>Manchester City v Chelsea</t>
+  </si>
+  <si>
+    <t>15/01/2022 15:00 | Premier League</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>Manchester City v Brentford</t>
+  </si>
+  <si>
+    <t>09/02/2022 20:00 | Premier League</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>Manchester City v Tottenham Hotspur</t>
+  </si>
+  <si>
+    <t>19/02/2022 15:00 | Premier League</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>Manchester City v Manchester United</t>
+  </si>
+  <si>
+    <t>05/03/2022 15:00 | Premier League</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manchester City v Brighton &amp; Hove Albion </t>
+  </si>
+  <si>
+    <t>19/03/2022 15:00 | Premier League</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manchester City v Liverpool </t>
+  </si>
+  <si>
+    <t>09/04/2022 15:00 | Premier League</t>
+  </si>
+  <si>
     <t>55</t>
   </si>
   <si>
-    <t xml:space="preserve">Manchester City v Southampton </t>
-  </si>
-  <si>
-    <t>18/09/2021 15:00 | Premier League</t>
-  </si>
-  <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>Manchester City v Wycombe Wanderers</t>
-  </si>
-  <si>
-    <t>21/09/2021 19:45 | Carabao Cup</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>Chelsea v Manchester City</t>
-  </si>
-  <si>
-    <t>25/09/2021 12:30 | Premier League</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>Manchester City v Burnley</t>
-  </si>
-  <si>
-    <t>16/10/2021 15:00 | Premier League</t>
-  </si>
-  <si>
-    <t>57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manchester City v Crystal Palace </t>
-  </si>
-  <si>
-    <t>30/10/2021 15:00 | Premier League</t>
-  </si>
-  <si>
-    <t>58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manchester City v Everton </t>
-  </si>
-  <si>
-    <t>20/11/2021 15:00 | Premier League</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>Manchester City v West Ham United</t>
-  </si>
-  <si>
-    <t>27/11/2021 15:00 | Premier League</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>Manchester City v Wolverhampton Wanderers</t>
-  </si>
-  <si>
-    <t>11/12/2021 15:00 | Premier League</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manchester City v Leeds United </t>
-  </si>
-  <si>
-    <t>15/12/2021 20:00 | Premier League</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>Manchester City v Leicester City</t>
-  </si>
-  <si>
-    <t>26/12/2021 15:00 | Premier League</t>
-  </si>
-  <si>
-    <t>Manchester City v Chelsea</t>
-  </si>
-  <si>
-    <t>15/01/2022 15:00 | Premier League</t>
-  </si>
-  <si>
-    <t>Manchester City v Brentford</t>
-  </si>
-  <si>
-    <t>09/02/2022 20:00 | Premier League</t>
-  </si>
-  <si>
-    <t>Manchester City v Tottenham Hotspur</t>
-  </si>
-  <si>
-    <t>19/02/2022 15:00 | Premier League</t>
-  </si>
-  <si>
-    <t>Manchester City v Manchester United</t>
-  </si>
-  <si>
-    <t>05/03/2022 15:00 | Premier League</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manchester City v Brighton &amp; Hove Albion </t>
-  </si>
-  <si>
-    <t>19/03/2022 15:00 | Premier League</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manchester City v Liverpool </t>
-  </si>
-  <si>
-    <t>09/04/2022 15:00 | Premier League</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>Manchester City v Watford</t>
   </si>
   <si>
@@ -166,13 +175,13 @@
     <t>07/05/2022 15:00 | Premier League</t>
   </si>
   <si>
+    <t>46</t>
+  </si>
+  <si>
     <t>Manchester City v Aston Villa</t>
   </si>
   <si>
     <t>22/05/2022 15:00 | Premier League</t>
-  </si>
-  <si>
-    <t>51</t>
   </si>
 </sst>
 </file>
@@ -595,51 +604,51 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -650,84 +659,84 @@
         <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>